<commit_message>
set up test data for contacts form
</commit_message>
<xml_diff>
--- a/src/main/java/com/company/app/testdata/data.xlsx
+++ b/src/main/java/com/company/app/testdata/data.xlsx
@@ -24,6 +24,85 @@
     </ext>
   </extLst>
 </workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
+  <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t>email</t>
+  </si>
+  <si>
+    <t>phone</t>
+  </si>
+  <si>
+    <t>message</t>
+  </si>
+  <si>
+    <t>alpha@test.com</t>
+  </si>
+  <si>
+    <t>+372100000</t>
+  </si>
+  <si>
+    <t>Inform about your new office</t>
+  </si>
+  <si>
+    <t>beta@test.com</t>
+  </si>
+  <si>
+    <t>78787878</t>
+  </si>
+  <si>
+    <t>All is well !!</t>
+  </si>
+  <si>
+    <t>000000000000</t>
+  </si>
+  <si>
+    <t>Zero Valid</t>
+  </si>
+  <si>
+    <t>zero@test.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">So feel been kept be at gate. Be september it extensive oh concluded of certainty. In read most gate at body held it ever no. Talking justice welcome message inquiry in started of am me. Led own hearted highest visited lasting sir through compass his. Guest tiled he quick by so these trees am. It announcing alteration at surrounded comparison. 
+So insisted received is occasion advanced honoured. Among ready to which up. Attacks smiling and may out assured moments man nothing outward. Thrown any behind afford either the set depend one temper. Instrument melancholy in acceptance collecting frequently be if. Zealously now pronounce existence add you instantly say offending. Merry their far had widen was. Concerns no in expenses raillery formerly. 
+Brother set had private his letters observe outward resolve. Shutters ye marriage to throwing we as. Effect in if agreed he wished wanted admire expect. Or shortly visitor is comfort placing to cheered do. Few hills tears are weeks saw. Partiality insensible celebrated is in. Am offended as wandered thoughts greatest an friendly. Evening covered in he exposed fertile to. Horses seeing at played plenty nature to expect we. Young say led stood hills own thing get. </t>
+  </si>
+  <si>
+    <t>Alpha Romeo</t>
+  </si>
+  <si>
+    <t>Beta Juliet</t>
+  </si>
+  <si>
+    <t>Negative test1</t>
+  </si>
+  <si>
+    <t>neg1@test.com</t>
+  </si>
+  <si>
+    <t>Hi Hello world</t>
+  </si>
+  <si>
+    <t>neg2@test.com</t>
+  </si>
+  <si>
+    <t>1234567</t>
+  </si>
+  <si>
+    <t>Negative test3</t>
+  </si>
+  <si>
+    <t>neg3@test.com</t>
+  </si>
+  <si>
+    <t>+475878910</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -80,14 +159,18 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="1" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -369,49 +452,126 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I3"/>
+  <dimension ref="A1:I7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A21" sqref="A21"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.25" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="16.25" customWidth="1"/>
-    <col min="2" max="2" width="14.33203125" customWidth="1"/>
-    <col min="3" max="3" width="30.08203125" customWidth="1"/>
-    <col min="4" max="4" width="15.75" customWidth="1"/>
+    <col min="2" max="2" width="18.33203125" customWidth="1"/>
+    <col min="3" max="3" width="18.1640625" customWidth="1"/>
+    <col min="4" max="4" width="48.1640625" customWidth="1"/>
     <col min="5" max="5" width="31.1640625" customWidth="1"/>
     <col min="6" max="6" width="14.33203125" customWidth="1"/>
     <col min="7" max="7" width="21.5" customWidth="1"/>
-    <col min="8" max="8" width="16" style="5" customWidth="1"/>
+    <col min="8" max="8" width="16" style="4" customWidth="1"/>
     <col min="9" max="9" width="35.33203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A1" s="1"/>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
-      <c r="G1" s="1"/>
-      <c r="H1" s="4"/>
-      <c r="I1" s="1"/>
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="H1"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="D2" s="2"/>
-      <c r="F2" s="3"/>
-      <c r="H2" s="6"/>
-      <c r="I2" s="3"/>
+      <c r="A2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="H2"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" t="s">
+        <v>9</v>
+      </c>
       <c r="F3" s="3"/>
-      <c r="H3" s="6"/>
+      <c r="H3" s="5"/>
       <c r="I3" s="3"/>
     </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="D4" s="8" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="B6" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C6" s="7" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>21</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C7" s="7" t="s">
+        <v>23</v>
+      </c>
+    </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B2" r:id="rId1"/>
+    <hyperlink ref="B3" r:id="rId2"/>
+    <hyperlink ref="B4" r:id="rId3"/>
+    <hyperlink ref="B5" r:id="rId4"/>
+    <hyperlink ref="B6" r:id="rId5"/>
+    <hyperlink ref="B7" r:id="rId6"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId7"/>
 </worksheet>
 </file>
</xml_diff>